<commit_message>
Aggiornate User Stories per includere la gestione delle spese
</commit_message>
<xml_diff>
--- a/User Stories/ISW Cards.xlsx
+++ b/User Stories/ISW Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita\ISW\progettoISW\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5615EA89-B9D1-40A2-8C61-DAB2EF5C74E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7FB1C-67F9-4A68-B208-5EB8E2BB528E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>TA:</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>L'utente dalla è lista dei viaggi clicca sul tasto "Visualizza i dettagli" del viaggio di cui vuole vedere i dettagli dalla lista dei viaggi a cui partecipa, dalla pagina che viene aperta può visualizzare le date del viaggio, i partecipanti e le tappe dell'itinerario</t>
+  </si>
+  <si>
+    <t>Titolo: Aggiugnere spesa la viaggio</t>
+  </si>
+  <si>
+    <t>L'utente clicca sul tasto "Visualizza i dettagli" del viaggio a cui desidera aggiungere una spesa dalla lista dei viaggi a cui partecipa, dalla pagina  che viene aperta può cliccare il tasto "gestisci spese" per aprire la pagina  in cui può aggiugnere o rimuovere le spese del viaggio e ottenerne sia il costo totale che il costo per persona, se si prova ad aggiungere una spesa con valori non validi si riceve un messaggio di avvertimento e si possono riinserire i dati</t>
   </si>
 </sst>
 </file>
@@ -441,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +646,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -648,7 +654,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -680,7 +686,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
@@ -692,7 +698,7 @@
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -712,7 +718,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -720,7 +726,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1202,7 +1208,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>21</v>
       </c>
@@ -1211,16 +1217,30 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -1233,16 +1253,34 @@
         <v>1</v>
       </c>
       <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
@@ -1251,82 +1289,140 @@
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="A49:F50"/>
-    <mergeCell ref="A51:B52"/>
-    <mergeCell ref="C51:D52"/>
-    <mergeCell ref="E51:F52"/>
-    <mergeCell ref="A53:F60"/>
-    <mergeCell ref="A17:F24"/>
-    <mergeCell ref="A5:F12"/>
-    <mergeCell ref="G5:L12"/>
-    <mergeCell ref="G17:L24"/>
-    <mergeCell ref="G13:L14"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:F16"/>
+  <mergeCells count="50">
+    <mergeCell ref="G49:L50"/>
+    <mergeCell ref="G51:H52"/>
+    <mergeCell ref="I51:J52"/>
+    <mergeCell ref="K51:L52"/>
+    <mergeCell ref="G53:L60"/>
+    <mergeCell ref="G37:L38"/>
+    <mergeCell ref="G39:H40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="K39:L40"/>
+    <mergeCell ref="G41:L48"/>
+    <mergeCell ref="A37:F38"/>
+    <mergeCell ref="A39:B40"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="E39:F40"/>
+    <mergeCell ref="A41:F48"/>
+    <mergeCell ref="G25:L26"/>
+    <mergeCell ref="G27:H28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="G29:L36"/>
+    <mergeCell ref="A25:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A29:F36"/>
     <mergeCell ref="G1:L2"/>
     <mergeCell ref="G3:H4"/>
     <mergeCell ref="I3:J4"/>
@@ -1335,26 +1431,23 @@
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="E3:F4"/>
-    <mergeCell ref="A25:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="A29:F36"/>
-    <mergeCell ref="G25:L26"/>
-    <mergeCell ref="G27:H28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="K27:L28"/>
-    <mergeCell ref="G29:L36"/>
-    <mergeCell ref="A37:F38"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="E39:F40"/>
-    <mergeCell ref="A41:F48"/>
-    <mergeCell ref="G37:L38"/>
-    <mergeCell ref="G39:H40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="K39:L40"/>
-    <mergeCell ref="G41:L48"/>
+    <mergeCell ref="G17:L24"/>
+    <mergeCell ref="A5:F12"/>
+    <mergeCell ref="G5:L12"/>
+    <mergeCell ref="A17:F24"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:L14"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="A49:F50"/>
+    <mergeCell ref="A51:B52"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="E51:F52"/>
+    <mergeCell ref="A53:F60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiornamento User Stories e inizio test di accettazione
</commit_message>
<xml_diff>
--- a/User Stories/ISW Cards.xlsx
+++ b/User Stories/ISW Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita\ISW\progettoISW\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7FB1C-67F9-4A68-B208-5EB8E2BB528E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFFAEBB-2622-4944-B567-6B5881714937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>TA:</t>
-  </si>
-  <si>
-    <t>Punti-storia:</t>
   </si>
   <si>
     <t>Titolo: Registrazione</t>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>L'utente clicca sul tasto "Visualizza i dettagli" del viaggio a cui desidera aggiungere una spesa dalla lista dei viaggi a cui partecipa, dalla pagina  che viene aperta può cliccare il tasto "gestisci spese" per aprire la pagina  in cui può aggiugnere o rimuovere le spese del viaggio e ottenerne sia il costo totale che il costo per persona, se si prova ad aggiungere una spesa con valori non validi si riceve un messaggio di avvertimento e si possono riinserire i dati</t>
+  </si>
+  <si>
+    <t>Punti-storia: 2</t>
+  </si>
+  <si>
+    <t>Punti-storia: 1</t>
   </si>
 </sst>
 </file>
@@ -447,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +461,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -466,7 +469,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -494,11 +497,11 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
@@ -506,11 +509,11 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -530,7 +533,7 @@
     </row>
     <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -538,7 +541,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -646,7 +649,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -654,7 +657,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -682,11 +685,11 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
@@ -694,11 +697,11 @@
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -718,7 +721,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -726,7 +729,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -834,7 +837,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -842,7 +845,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -870,11 +873,11 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
@@ -882,11 +885,11 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="L27" s="2"/>
     </row>
@@ -906,7 +909,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -914,7 +917,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1030,7 +1033,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1058,11 +1061,11 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
@@ -1070,11 +1073,11 @@
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L39" s="2"/>
     </row>
@@ -1094,7 +1097,7 @@
     </row>
     <row r="41" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1102,7 +1105,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -1210,7 +1213,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1218,7 +1221,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -1246,11 +1249,11 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2" t="s">
@@ -1258,11 +1261,11 @@
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L51" s="2"/>
     </row>
@@ -1282,7 +1285,7 @@
     </row>
     <row r="53" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1290,7 +1293,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -1450,5 +1453,6 @@
     <mergeCell ref="A53:F60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finita tabella risultati test di accettazione
</commit_message>
<xml_diff>
--- a/User Stories/ISW Cards.xlsx
+++ b/User Stories/ISW Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universita\ISW\progettoISW\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFFAEBB-2622-4944-B567-6B5881714937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1FDC5D-39F3-41CA-B484-2D347A667835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
-  <si>
-    <t>TA:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Titolo: Registrazione</t>
   </si>
@@ -97,9 +94,6 @@
     <t>L'utente dalla è lista dei viaggi clicca sul tasto "Visualizza i dettagli" del viaggio di cui vuole vedere i dettagli dalla lista dei viaggi a cui partecipa, dalla pagina che viene aperta può visualizzare le date del viaggio, i partecipanti e le tappe dell'itinerario</t>
   </si>
   <si>
-    <t>Titolo: Aggiugnere spesa la viaggio</t>
-  </si>
-  <si>
     <t>L'utente clicca sul tasto "Visualizza i dettagli" del viaggio a cui desidera aggiungere una spesa dalla lista dei viaggi a cui partecipa, dalla pagina  che viene aperta può cliccare il tasto "gestisci spese" per aprire la pagina  in cui può aggiugnere o rimuovere le spese del viaggio e ottenerne sia il costo totale che il costo per persona, se si prova ad aggiungere una spesa con valori non validi si riceve un messaggio di avvertimento e si possono riinserire i dati</t>
   </si>
   <si>
@@ -107,6 +101,39 @@
   </si>
   <si>
     <t>Punti-storia: 1</t>
+  </si>
+  <si>
+    <t>TA: register</t>
+  </si>
+  <si>
+    <t>TA: login</t>
+  </si>
+  <si>
+    <t>TA: mytravel</t>
+  </si>
+  <si>
+    <t>TA: form_modify_travel</t>
+  </si>
+  <si>
+    <t>TA: send_invite</t>
+  </si>
+  <si>
+    <t>TA: create_travel</t>
+  </si>
+  <si>
+    <t>TA: logout</t>
+  </si>
+  <si>
+    <t>TA: write_comment</t>
+  </si>
+  <si>
+    <t>TA: details_travel</t>
+  </si>
+  <si>
+    <t>TA: form_expense</t>
+  </si>
+  <si>
+    <t>Titolo: Aggiungere spesa la viaggio</t>
   </si>
 </sst>
 </file>
@@ -451,7 +478,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="G15" sqref="G15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -469,7 +496,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -493,27 +520,27 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -533,7 +560,7 @@
     </row>
     <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -541,7 +568,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -649,7 +676,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -657,7 +684,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -681,27 +708,27 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -712,8 +739,8 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -721,7 +748,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -729,7 +756,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -837,7 +864,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -845,7 +872,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -869,27 +896,27 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L27" s="2"/>
     </row>
@@ -909,7 +936,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -917,7 +944,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1025,7 +1052,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1033,7 +1060,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1057,27 +1084,27 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L39" s="2"/>
     </row>
@@ -1097,7 +1124,7 @@
     </row>
     <row r="41" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1105,7 +1132,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -1213,7 +1240,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1221,7 +1248,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -1245,27 +1272,27 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L51" s="2"/>
     </row>
@@ -1285,7 +1312,7 @@
     </row>
     <row r="53" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1293,7 +1320,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -1401,39 +1428,11 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="G49:L50"/>
-    <mergeCell ref="G51:H52"/>
-    <mergeCell ref="I51:J52"/>
-    <mergeCell ref="K51:L52"/>
-    <mergeCell ref="G53:L60"/>
-    <mergeCell ref="G37:L38"/>
-    <mergeCell ref="G39:H40"/>
-    <mergeCell ref="I39:J40"/>
-    <mergeCell ref="K39:L40"/>
-    <mergeCell ref="G41:L48"/>
-    <mergeCell ref="A37:F38"/>
-    <mergeCell ref="A39:B40"/>
-    <mergeCell ref="C39:D40"/>
-    <mergeCell ref="E39:F40"/>
-    <mergeCell ref="A41:F48"/>
-    <mergeCell ref="G25:L26"/>
-    <mergeCell ref="G27:H28"/>
-    <mergeCell ref="I27:J28"/>
-    <mergeCell ref="K27:L28"/>
-    <mergeCell ref="G29:L36"/>
-    <mergeCell ref="A25:F26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="A29:F36"/>
-    <mergeCell ref="G1:L2"/>
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="A49:F50"/>
+    <mergeCell ref="A51:B52"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="E51:F52"/>
+    <mergeCell ref="A53:F60"/>
     <mergeCell ref="G17:L24"/>
     <mergeCell ref="A5:F12"/>
     <mergeCell ref="G5:L12"/>
@@ -1446,11 +1445,39 @@
     <mergeCell ref="G15:H16"/>
     <mergeCell ref="I15:J16"/>
     <mergeCell ref="K15:L16"/>
-    <mergeCell ref="A49:F50"/>
-    <mergeCell ref="A51:B52"/>
-    <mergeCell ref="C51:D52"/>
-    <mergeCell ref="E51:F52"/>
-    <mergeCell ref="A53:F60"/>
+    <mergeCell ref="G1:L2"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="I3:J4"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="A25:F26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="A29:F36"/>
+    <mergeCell ref="G25:L26"/>
+    <mergeCell ref="G27:H28"/>
+    <mergeCell ref="I27:J28"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="G29:L36"/>
+    <mergeCell ref="A37:F38"/>
+    <mergeCell ref="A39:B40"/>
+    <mergeCell ref="C39:D40"/>
+    <mergeCell ref="E39:F40"/>
+    <mergeCell ref="A41:F48"/>
+    <mergeCell ref="G37:L38"/>
+    <mergeCell ref="G39:H40"/>
+    <mergeCell ref="I39:J40"/>
+    <mergeCell ref="K39:L40"/>
+    <mergeCell ref="G41:L48"/>
+    <mergeCell ref="G49:L50"/>
+    <mergeCell ref="G51:H52"/>
+    <mergeCell ref="I51:J52"/>
+    <mergeCell ref="K51:L52"/>
+    <mergeCell ref="G53:L60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>